<commit_message>
- fix number inputs
 - refactor code
</commit_message>
<xml_diff>
--- a/public/excel/Dose_rate.xlsx
+++ b/public/excel/Dose_rate.xlsx
@@ -224,14 +224,14 @@
                 <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
                 <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
               </a:rPr>
-              <a:t>Radication chemistry</a:t>
+              <a:t>Dose</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0">
                 <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
                 <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
               </a:rPr>
-              <a:t> yield</a:t>
+              <a:t> rate</a:t>
             </a:r>
             <a:endParaRPr lang="en-US">
               <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
@@ -329,11 +329,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="91849088"/>
-        <c:axId val="91851008"/>
+        <c:axId val="88244608"/>
+        <c:axId val="88246528"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="91849088"/>
+        <c:axId val="88244608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -396,12 +396,12 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91851008"/>
+        <c:crossAx val="88246528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="91851008"/>
+        <c:axId val="88246528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -465,7 +465,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91849088"/>
+        <c:crossAx val="88244608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -807,7 +807,7 @@
   <dimension ref="B2:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>